<commit_message>
updt : Tugas Kerkom2
</commit_message>
<xml_diff>
--- a/Tugas Kerkom2/Kelompok_4.xlsx
+++ b/Tugas Kerkom2/Kelompok_4.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>i</t>
   </si>
@@ -81,6 +81,9 @@
   <si>
     <t>e = 0,00001</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
 </sst>
 </file>
 
@@ -89,7 +92,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,8 +116,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +155,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -158,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -189,7 +211,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -200,11 +221,37 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -222,6 +269,1878 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Secant!$C$17:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Secant!$D$17:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-12658.850000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4094.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-946.49000000000012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-118.91000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-7.9700000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-6.35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.7299999999999986</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>106.21000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>933.79000000000008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4081.3300000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12646.150000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1943515488"/>
+        <c:axId val="-1943522560"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1943515488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1943522560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1943522560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1943515488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Secant!$C$17:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Secant!$D$17:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-12658.850000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4094.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-946.49000000000012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-118.91000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-7.9700000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-6.35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.7299999999999986</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>106.21000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>933.79000000000008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4081.3300000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12646.150000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-147243760"/>
+        <c:axId val="-147242672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-147243760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-147242672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-147242672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-147243760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>479425</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -487,21 +2406,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="39.6328125" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>6</v>
-      </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -513,15 +2430,12 @@
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="5" t="s">
-        <v>11</v>
+      <c r="A4" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -546,22 +2460,19 @@
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="4">
         <v>0</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>1</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <f xml:space="preserve"> (4.15*(E5^5)) - (2.53*(E5^3)) - 6.35</f>
         <v>-4.7299999999999986</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="14">
         <f>(20.75*(E5^4)) - (7.59*(E5^2))</f>
         <v>13.16</v>
       </c>
@@ -572,55 +2483,57 @@
       <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="8"/>
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="9">
         <v>1</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="15">
         <f xml:space="preserve"> E5 - (F5/G5)</f>
         <v>1.3594224924012157</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="15">
         <f t="shared" ref="F6:F10" si="0" xml:space="preserve"> (4.15*(E6^5)) - (2.53*(E6^3)) - 6.35</f>
         <v>6.5612777302011214</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="15">
         <f t="shared" ref="G6:G10" si="1">(20.75*(E6^4)) - (7.59*(E6^2))</f>
         <v>56.839127414780748</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="16">
         <f t="shared" ref="H6:H10" si="2">F6/G6</f>
         <v>0.11543593346042276</v>
       </c>
-      <c r="I6" s="17">
-        <f>ABS(E6-E5)</f>
+      <c r="I6" s="16">
+        <f t="shared" ref="I6:I11" si="3">ABS(E6-E5)</f>
         <v>0.35942249240121571</v>
       </c>
       <c r="J6" s="10" t="b">
-        <f>I6&lt;0.00001</f>
+        <f t="shared" ref="J6:J11" si="4">I6&lt;0.00001</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
-        <v>13</v>
+      <c r="A7" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="4">
         <v>2</v>
       </c>
-      <c r="E7" s="15">
-        <f t="shared" ref="E7:E9" si="3" xml:space="preserve"> E6 - (F6/G6)</f>
+      <c r="E7" s="14">
+        <f t="shared" ref="E7:E9" si="5" xml:space="preserve"> E6 - (F6/G6)</f>
         <v>1.243986558940793</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <f t="shared" si="0"/>
         <v>1.1426427916781297</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="14">
         <f t="shared" si="1"/>
         <v>37.945812097114249</v>
       </c>
@@ -629,58 +2542,62 @@
         <v>3.0112487479613773E-2</v>
       </c>
       <c r="I7" s="13">
-        <f>ABS(E7-E6)</f>
+        <f t="shared" si="3"/>
         <v>0.11543593346042269</v>
       </c>
       <c r="J7" s="10" t="b">
-        <f>I7&lt;0.00001</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="9">
         <v>3</v>
       </c>
-      <c r="E8" s="16">
-        <f t="shared" si="3"/>
+      <c r="E8" s="15">
+        <f t="shared" si="5"/>
         <v>1.2138740714611793</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="15">
         <f t="shared" si="0"/>
         <v>6.2216795467798569E-2</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="15">
         <f t="shared" si="1"/>
         <v>33.868060085782346</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="16">
         <f t="shared" si="2"/>
         <v>1.8370345189601483E-3</v>
       </c>
-      <c r="I8" s="17">
-        <f>ABS(E8-E7)</f>
+      <c r="I8" s="16">
+        <f t="shared" si="3"/>
         <v>3.0112487479613703E-2</v>
       </c>
       <c r="J8" s="10" t="b">
-        <f>I8&lt;0.00001</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="8"/>
       <c r="D9" s="4">
         <v>4</v>
       </c>
-      <c r="E9" s="15">
-        <f t="shared" si="3"/>
+      <c r="E9" s="14">
+        <f t="shared" si="5"/>
         <v>1.2120370369422191</v>
       </c>
-      <c r="F9" s="15">
-        <f t="shared" si="0"/>
+      <c r="F9" s="14">
+        <f xml:space="preserve"> (4.15*(E9^5)) - (2.53*(E9^3)) - 6.35</f>
         <v>2.1904241597603402E-4</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <f t="shared" si="1"/>
         <v>33.629783672845292</v>
       </c>
@@ -689,61 +2606,182 @@
         <v>6.5133459705511581E-6</v>
       </c>
       <c r="I9" s="13">
-        <f>ABS(E9-E8)</f>
+        <f t="shared" si="3"/>
         <v>1.8370345189602233E-3</v>
       </c>
       <c r="J9" s="10" t="b">
-        <f>I9&lt;0.00001</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="D10" s="9">
+      <c r="A10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="24">
         <v>5</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="25">
         <f xml:space="preserve"> E9 - (F9/G9)</f>
         <v>1.2120305235962485</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="25">
         <f t="shared" si="0"/>
         <v>2.7444722050518067E-9</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="25">
         <f t="shared" si="1"/>
         <v>33.628940952865619</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="26">
         <f t="shared" si="2"/>
         <v>8.1610426236688921E-11</v>
       </c>
-      <c r="I10" s="17">
-        <f>ABS(E10-E9)</f>
+      <c r="I10" s="26">
+        <f t="shared" si="3"/>
         <v>6.5133459705712937E-6</v>
       </c>
-      <c r="J10" s="10" t="b">
-        <f>I10&lt;0.00001</f>
+      <c r="J10" s="27" t="b">
+        <f t="shared" si="4"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D11" s="4"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="23"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D14" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D15" s="11">
+        <v>-5</v>
+      </c>
+      <c r="E15" s="11">
+        <f>(4.15*(D15^5)) - (2.53*(D15^3)) - 6.35</f>
+        <v>-12658.850000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D16" s="11">
+        <v>-4</v>
+      </c>
+      <c r="E16" s="11">
+        <f t="shared" ref="E16:E25" si="6">(4.15*(D16^5)) - (2.53*(D16^3)) - 6.35</f>
+        <v>-4094.03</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D17" s="11">
+        <v>-3</v>
+      </c>
+      <c r="E17" s="11">
+        <f t="shared" si="6"/>
+        <v>-946.49000000000012</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D18" s="11">
+        <v>-2</v>
+      </c>
+      <c r="E18" s="11">
+        <f t="shared" si="6"/>
+        <v>-118.91000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="E19" s="11">
+        <f t="shared" si="6"/>
+        <v>-7.9700000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D20" s="11">
+        <v>0</v>
+      </c>
+      <c r="E20" s="11">
+        <f t="shared" si="6"/>
+        <v>-6.35</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D21" s="20">
+        <v>1</v>
+      </c>
+      <c r="E21" s="20">
+        <f t="shared" si="6"/>
+        <v>-4.7299999999999986</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D22" s="20">
+        <v>2</v>
+      </c>
+      <c r="E22" s="20">
+        <f t="shared" si="6"/>
+        <v>106.21000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D23" s="11">
+        <v>3</v>
+      </c>
+      <c r="E23" s="11">
+        <f t="shared" si="6"/>
+        <v>933.79000000000008</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D24" s="11">
+        <v>4</v>
+      </c>
+      <c r="E24" s="11">
+        <f t="shared" si="6"/>
+        <v>4081.3300000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D25" s="11">
+        <v>5</v>
+      </c>
+      <c r="E25" s="11">
+        <f t="shared" si="6"/>
+        <v>12646.150000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C16" sqref="C16:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="34.54296875" customWidth="1"/>
-    <col min="4" max="4" width="16.36328125" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.08984375" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
     <col min="6" max="6" width="10.08984375" customWidth="1"/>
     <col min="7" max="7" width="11.81640625" customWidth="1"/>
   </cols>
@@ -757,16 +2795,16 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="19" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="11"/>
@@ -779,10 +2817,10 @@
       <c r="C4" s="11">
         <v>0</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="21">
         <v>1</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="21">
         <f xml:space="preserve"> (4.15*(D4^5)) - (2.53*(D4^3)) - 6.35</f>
         <v>-4.7299999999999986</v>
       </c>
@@ -791,21 +2829,21 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <v>1</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="22">
         <v>2</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="22">
         <f xml:space="preserve"> (4.15*(D5^5)) - (2.53*(D5^3)) - 6.35</f>
         <v>106.21000000000002</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="18">
         <f>ABS(D5-D4)</f>
         <v>1</v>
       </c>
-      <c r="G5" s="18" t="b">
+      <c r="G5" s="17" t="b">
         <f>F5&lt;0.0001</f>
         <v>0</v>
       </c>
@@ -817,11 +2855,11 @@
       <c r="C6" s="11">
         <v>2</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="21">
         <f>D5-((E5)*(D4-D5)/(E4-E5))</f>
         <v>1.0426356589147288</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="21">
         <f xml:space="preserve"> (4.15*(D6^5)) - (2.53*(D6^3)) - 6.35</f>
         <v>-4.1041837049303274</v>
       </c>
@@ -835,22 +2873,22 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C7" s="18">
+      <c r="C7" s="17">
         <v>3</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="22">
         <f t="shared" ref="D7:D12" si="2">D6-((E6)*(D5-D6)/(E5-E6))</f>
         <v>1.0782539175683339</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="22">
         <f t="shared" ref="E7:E12" si="3" xml:space="preserve"> (4.15*(D7^5)) - (2.53*(D7^3)) - 6.35</f>
         <v>-3.4730598274020807</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="18">
         <f t="shared" si="0"/>
         <v>3.5618258653605128E-2</v>
       </c>
-      <c r="G7" s="18" t="b">
+      <c r="G7" s="17" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -859,11 +2897,11 @@
       <c r="C8" s="11">
         <v>4</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="21">
         <f t="shared" si="2"/>
         <v>1.2742603556963479</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="21">
         <f t="shared" si="3"/>
         <v>2.3577064511031249</v>
       </c>
@@ -877,22 +2915,22 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <v>5</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="22">
         <f t="shared" si="2"/>
         <v>1.1950039386906166</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="22">
         <f t="shared" si="3"/>
         <v>-0.55411806364760974</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="18">
         <f t="shared" si="0"/>
         <v>7.9256417005731272E-2</v>
       </c>
-      <c r="G9" s="18" t="b">
+      <c r="G9" s="17" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -901,11 +2939,11 @@
       <c r="C10" s="11">
         <v>6</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="21">
         <f t="shared" si="2"/>
         <v>1.2100863765574545</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="21">
         <f t="shared" si="3"/>
         <v>-6.5135518372514412E-2</v>
       </c>
@@ -919,43 +2957,43 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C11" s="18">
+      <c r="C11" s="17">
         <v>7</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="22">
         <f t="shared" si="2"/>
         <v>1.2120954511517736</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="22">
         <f t="shared" si="3"/>
         <v>2.1837204029164781E-3</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="18">
         <f t="shared" si="0"/>
         <v>2.0090745943190935E-3</v>
       </c>
-      <c r="G11" s="18" t="b">
+      <c r="G11" s="17" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C12" s="11">
+      <c r="C12" s="28">
         <v>8</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="29">
         <f t="shared" si="2"/>
         <v>1.2120302802249716</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="29">
         <f t="shared" si="3"/>
         <v>-8.1815699974896461E-6</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="30">
         <f t="shared" si="0"/>
         <v>6.5170926802027296E-5</v>
       </c>
-      <c r="G12" s="11" t="b">
+      <c r="G12" s="28" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -967,16 +3005,121 @@
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C16" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C17" s="11">
+        <v>-5</v>
+      </c>
+      <c r="D17" s="11">
+        <f>(4.15*(C17^5)) - (2.53*(C17^3)) - 6.35</f>
+        <v>-12658.850000000002</v>
+      </c>
       <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C18" s="11">
+        <v>-4</v>
+      </c>
+      <c r="D18" s="11">
+        <f t="shared" ref="D18:D27" si="4">(4.15*(C18^5)) - (2.53*(C18^3)) - 6.35</f>
+        <v>-4094.03</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C19" s="11">
+        <v>-3</v>
+      </c>
+      <c r="D19" s="11">
+        <f t="shared" si="4"/>
+        <v>-946.49000000000012</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C20" s="11">
+        <v>-2</v>
+      </c>
+      <c r="D20" s="11">
+        <f t="shared" si="4"/>
+        <v>-118.91000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="D21" s="11">
+        <f t="shared" si="4"/>
+        <v>-7.9700000000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C22" s="11">
+        <v>0</v>
+      </c>
+      <c r="D22" s="11">
+        <f t="shared" si="4"/>
+        <v>-6.35</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C23" s="20">
+        <v>1</v>
+      </c>
+      <c r="D23" s="20">
+        <f t="shared" si="4"/>
+        <v>-4.7299999999999986</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C24" s="20">
+        <v>2</v>
+      </c>
+      <c r="D24" s="20">
+        <f t="shared" si="4"/>
+        <v>106.21000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C25" s="11">
+        <v>3</v>
+      </c>
+      <c r="D25" s="11">
+        <f t="shared" si="4"/>
+        <v>933.79000000000008</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C26" s="11">
+        <v>4</v>
+      </c>
+      <c r="D26" s="11">
+        <f t="shared" si="4"/>
+        <v>4081.3300000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C27" s="11">
+        <v>5</v>
+      </c>
+      <c r="D27" s="11">
+        <f t="shared" si="4"/>
+        <v>12646.150000000001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>